<commit_message>
finis quelque bug sql
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16124824-FFEE-4FC3-84DB-62BC5247B8F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34363DEE-040C-4CA5-A9E5-E2C7BFD1F8D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,7 +392,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,9 +446,6 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
-      </c>
       <c r="B2">
         <v>22</v>
       </c>
@@ -481,6 +478,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12</v>
+      </c>
       <c r="B3">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Fix de l'update/insert et vérification du 0 que en idTrajet que t'avais pas fait !
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5596B17-D654-4082-BEA3-9E22D53FBECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5C888-E4EF-419F-820F-1570B5E8D5A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">id du client : </t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>Id du trajet</t>
+  </si>
+  <si>
+    <t>Etat du trajet</t>
+  </si>
+  <si>
+    <t>Etat du chauffeur</t>
+  </si>
+  <si>
+    <t>"Pas commencé"</t>
+  </si>
+  <si>
+    <t>"En cours"</t>
+  </si>
+  <si>
+    <t>"Finis"</t>
   </si>
 </sst>
 </file>
@@ -391,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,9 +425,11 @@
     <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -446,10 +463,16 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="B2">
         <v>555</v>
@@ -481,10 +504,16 @@
       <c r="K2">
         <v>8</v>
       </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>1002</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -516,10 +545,16 @@
       <c r="K3">
         <v>4</v>
       </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>22</v>
@@ -551,8 +586,14 @@
       <c r="K4">
         <v>1</v>
       </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>

<commit_message>
reste la fin de la remunération mais bon dodo
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5C888-E4EF-419F-820F-1570B5E8D5A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B80371-1D2E-421D-AB40-0BDF9C4BA3B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +598,21 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
je suis un génie arthur <3
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EACA990-554D-461D-9B8F-A56712A58A14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7684B15F-499A-43B9-AAA5-712B4A8408D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="n">
-        <v>2090.0</v>
+        <v>611.0</v>
       </c>
       <c r="B2">
         <v>555</v>
@@ -512,8 +512,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="n">
-        <v>2091.0</v>
+      <c r="A3">
+        <v>607</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -553,8 +553,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="n">
-        <v>2092.0</v>
+      <c r="A4">
+        <v>608</v>
       </c>
       <c r="B4">
         <v>22</v>

</xml_diff>

<commit_message>
d o n e
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7684B15F-499A-43B9-AAA5-712B4A8408D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CABEA3-0F60-4D0C-89C0-CD22A54A05A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chauffeur" sheetId="1" r:id="rId1"/>
+    <sheet name="Collab" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">id du client : </t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t>"Finis"</t>
+  </si>
+  <si>
+    <t>Id link</t>
+  </si>
+  <si>
+    <t>Id trajet</t>
+  </si>
+  <si>
+    <t>Id service</t>
+  </si>
+  <si>
+    <t>Id annex</t>
+  </si>
+  <si>
+    <t>Quantite</t>
+  </si>
+  <si>
+    <t>Statut</t>
+  </si>
+  <si>
+    <t>Date de début</t>
+  </si>
+  <si>
+    <t>Date de fin</t>
   </si>
 </sst>
 </file>
@@ -122,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -471,8 +497,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="n">
-        <v>611.0</v>
+      <c r="A2">
+        <v>611</v>
       </c>
       <c r="B2">
         <v>555</v>
@@ -617,4 +643,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650436FE-D25C-4178-82F6-E9FC428956D4}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="n">
+        <v>361.0</v>
+      </c>
+      <c r="B2">
+        <v>574</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fini je dirais les petits potes
</commit_message>
<xml_diff>
--- a/ExcelToBDD/excel.xlsx
+++ b/ExcelToBDD/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CABEA3-0F60-4D0C-89C0-CD22A54A05A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E54F4-C9C2-4CB7-B435-AB2E24EA5516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">id du client : </t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Date de fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id de la rémunération </t>
+  </si>
+  <si>
+    <t>id de la rémunération</t>
   </si>
 </sst>
 </file>
@@ -432,30 +438,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="15.7109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="19.140625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="1" width="18.42578125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="1" width="36.28515625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="20.42578125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="21.5703125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="18.140625" collapsed="false"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -495,16 +502,19 @@
       <c r="M1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="B2">
         <v>555</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>44114.416666666664</v>
@@ -536,16 +546,19 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>44112.583333333336</v>
@@ -577,16 +590,19 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>608</v>
+        <v>623</v>
       </c>
       <c r="B4">
         <v>22</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
         <v>44114.416666666664</v>
@@ -618,23 +634,26 @@
       <c r="M4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
@@ -647,7 +666,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650436FE-D25C-4178-82F6-E9FC428956D4}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
@@ -655,10 +674,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -683,16 +703,19 @@
       <c r="H1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="n">
-        <v>361.0</v>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>362</v>
       </c>
       <c r="B2">
         <v>574</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -707,7 +730,68 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="H2" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="I2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>363</v>
+      </c>
+      <c r="B3">
+        <v>574</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="H3" s="3">
         <v>0.43055555555555558</v>
+      </c>
+      <c r="I3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>364</v>
+      </c>
+      <c r="B4">
+        <v>574</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="I4">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>